<commit_message>
adds automatic asset generator for GUI testing
</commit_message>
<xml_diff>
--- a/100runs/run001/NotionalETEOutput001.xlsx
+++ b/100runs/run001/NotionalETEOutput001.xlsx
@@ -49,13 +49,13 @@
     <t>tUp</t>
   </si>
   <si>
-    <t>Missile_HIGHWIND_State_Update</t>
+    <t>Missile_HELLMASKER_State_Update</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND_301.MISSILE_HIGHWIND_301</t>
+    <t>MISSILE_HELLMASKER_273.MISSILE_HELLMASKER_273</t>
   </si>
   <si>
-    <t>MISSILE_HIGHWIND</t>
+    <t>MISSILE_HELLMASKER</t>
   </si>
 </sst>
 </file>
@@ -471,22 +471,22 @@
         <v>152.142</v>
       </c>
       <c r="F2">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G2">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H2">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I2">
-        <v>-938.1746987304058</v>
+        <v>1114862.744020319</v>
       </c>
       <c r="J2">
-        <v>1543.168458045929</v>
+        <v>4843210.199881298</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>3984361.876623415</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -506,22 +506,22 @@
         <v>153.142</v>
       </c>
       <c r="F3">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G3">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H3">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I3">
-        <v>-919.6526320646877</v>
+        <v>1114892.358053615</v>
       </c>
       <c r="J3">
-        <v>1505.629659846657</v>
+        <v>4843161.548424403</v>
       </c>
       <c r="K3">
-        <v>336.8170207210867</v>
+        <v>3984665.671971521</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -541,22 +541,22 @@
         <v>154.142</v>
       </c>
       <c r="F4">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G4">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H4">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I4">
-        <v>-900.6744765473155</v>
+        <v>1114922.701305236</v>
       </c>
       <c r="J4">
-        <v>1468.090861647384</v>
+        <v>4843112.896967506</v>
       </c>
       <c r="K4">
-        <v>656.8388008752233</v>
+        <v>3984954.318691022</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -576,22 +576,22 @@
         <v>155.142</v>
       </c>
       <c r="F5">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G5">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H5">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I5">
-        <v>-881.2290014099107</v>
+        <v>1114953.791731514</v>
       </c>
       <c r="J5">
-        <v>1430.552063448112</v>
+        <v>4843064.245510611</v>
       </c>
       <c r="K5">
-        <v>960.0653404624122</v>
+        <v>3985227.816781918</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -611,22 +611,22 @@
         <v>156.142</v>
       </c>
       <c r="F6">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G6">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H6">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I6">
-        <v>-861.3046993367566</v>
+        <v>1114985.647730935</v>
       </c>
       <c r="J6">
-        <v>1393.01326524884</v>
+        <v>4843015.594053715</v>
       </c>
       <c r="K6">
-        <v>1246.496639482651</v>
+        <v>3985486.166244211</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -646,22 +646,22 @@
         <v>157.142</v>
       </c>
       <c r="F7">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G7">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H7">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I7">
-        <v>-840.8897796550724</v>
+        <v>1115018.288155036</v>
       </c>
       <c r="J7">
-        <v>1355.474467049568</v>
+        <v>4842966.942596819</v>
       </c>
       <c r="K7">
-        <v>1516.132697935943</v>
+        <v>3985729.367077899</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -681,22 +681,22 @@
         <v>158.142</v>
       </c>
       <c r="F8">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G8">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H8">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I8">
-        <v>-819.9721613576088</v>
+        <v>1115051.732319551</v>
       </c>
       <c r="J8">
-        <v>1317.935668850296</v>
+        <v>4842918.291139923</v>
       </c>
       <c r="K8">
-        <v>1768.973515822286</v>
+        <v>3985957.419282982</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -716,22 +716,22 @@
         <v>159.142</v>
       </c>
       <c r="F9">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G9">
-        <v>-113.8360154227634</v>
+        <v>4841128.632839935</v>
       </c>
       <c r="H9">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I9">
-        <v>-798.5394659534261</v>
+        <v>1115086.000015849</v>
       </c>
       <c r="J9">
-        <v>1280.396870651024</v>
+        <v>4842869.639683028</v>
       </c>
       <c r="K9">
-        <v>2005.01909314168</v>
+        <v>3986170.32285946</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -751,22 +751,22 @@
         <v>160.142</v>
       </c>
       <c r="F10">
-        <v>213.8975288704108</v>
+        <v>1116578.499706819</v>
       </c>
       <c r="G10">
-        <v>-95.03848500343847</v>
+        <v>4841145.145673027</v>
       </c>
       <c r="H10">
-        <v>965.2861550749826</v>
+        <v>3985231.243275555</v>
       </c>
       <c r="I10">
-        <v>-776.5790101426336</v>
+        <v>1115121.111522643</v>
       </c>
       <c r="J10">
-        <v>1242.858072451752</v>
+        <v>4842820.988226132</v>
       </c>
       <c r="K10">
-        <v>2224.269429894124</v>
+        <v>3986368.077807335</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -786,22 +786,22 @@
         <v>161.142</v>
       </c>
       <c r="F11">
-        <v>166.0094349316718</v>
+        <v>1116529.819143229</v>
       </c>
       <c r="G11">
-        <v>-76.24095458411352</v>
+        <v>4841161.658506118</v>
       </c>
       <c r="H11">
-        <v>1189.226047587963</v>
+        <v>3985430.497828071</v>
       </c>
       <c r="I11">
-        <v>-754.0777983107491</v>
+        <v>1115157.08761799</v>
       </c>
       <c r="J11">
-        <v>1205.31927425248</v>
+        <v>4842772.336769236</v>
       </c>
       <c r="K11">
-        <v>2426.724526079619</v>
+        <v>3986550.684126605</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -821,22 +821,22 @@
         <v>162.142</v>
       </c>
       <c r="F12">
-        <v>137.8775820687813</v>
+        <v>1116501.221754201</v>
       </c>
       <c r="G12">
-        <v>-57.4434241647886</v>
+        <v>4841178.17133921</v>
       </c>
       <c r="H12">
-        <v>1322.61610028959</v>
+        <v>3985549.184029814</v>
       </c>
       <c r="I12">
-        <v>-731.02251483824</v>
+        <v>1115193.949591588</v>
       </c>
       <c r="J12">
-        <v>1167.780476053207</v>
+        <v>4842723.68531234</v>
       </c>
       <c r="K12">
-        <v>2612.384381698167</v>
+        <v>3986718.141817271</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -856,22 +856,22 @@
         <v>163.142</v>
       </c>
       <c r="F13">
-        <v>120.1186926845775</v>
+        <v>1116483.168984236</v>
       </c>
       <c r="G13">
-        <v>-38.64589374546366</v>
+        <v>4841194.684172302</v>
       </c>
       <c r="H13">
-        <v>1417.940955466436</v>
+        <v>3985634.001036506</v>
       </c>
       <c r="I13">
-        <v>-707.3995162206917</v>
+        <v>1115231.719257372</v>
       </c>
       <c r="J13">
-        <v>1130.241677853935</v>
+        <v>4842675.033855444</v>
       </c>
       <c r="K13">
-        <v>2781.248996749766</v>
+        <v>3986870.450879332</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -891,22 +891,22 @@
         <v>164.142</v>
       </c>
       <c r="F14">
-        <v>107.7337153155978</v>
+        <v>1116470.579055744</v>
       </c>
       <c r="G14">
-        <v>-19.84836332613872</v>
+        <v>4841211.197005392</v>
       </c>
       <c r="H14">
-        <v>1492.170369122318</v>
+        <v>3985700.047994175</v>
       </c>
       <c r="I14">
-        <v>-683.1948229949469</v>
+        <v>1115270.41896643</v>
       </c>
       <c r="J14">
-        <v>1092.702879654663</v>
+        <v>4842626.382398549</v>
       </c>
       <c r="K14">
-        <v>2933.318371234416</v>
+        <v>3987007.611312789</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -926,22 +926,22 @@
         <v>165.142</v>
       </c>
       <c r="F15">
-        <v>98.49415131058404</v>
+        <v>1116461.186592062</v>
       </c>
       <c r="G15">
-        <v>-1.050832906813801</v>
+        <v>4841227.709838484</v>
       </c>
       <c r="H15">
-        <v>1552.970016664637</v>
+        <v>3985754.145575577</v>
       </c>
       <c r="I15">
-        <v>-658.3941114664276</v>
+        <v>1115310.071620219</v>
       </c>
       <c r="J15">
-        <v>1055.164081455391</v>
+        <v>4842577.730941653</v>
       </c>
       <c r="K15">
-        <v>3068.592505152117</v>
+        <v>3987129.623117641</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -961,22 +961,22 @@
         <v>166.142</v>
       </c>
       <c r="F16">
-        <v>91.27010252552427</v>
+        <v>1116453.842997082</v>
       </c>
       <c r="G16">
-        <v>17.74669751251114</v>
+        <v>4841244.222671575</v>
       </c>
       <c r="H16">
-        <v>1604.462879973819</v>
+        <v>3985799.962278091</v>
       </c>
       <c r="I16">
-        <v>-632.9827052327547</v>
+        <v>1115350.700684129</v>
       </c>
       <c r="J16">
-        <v>1017.625283256119</v>
+        <v>4842529.079484756</v>
       </c>
       <c r="K16">
-        <v>3187.071398502869</v>
+        <v>3987236.48629389</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -996,22 +996,22 @@
         <v>167.142</v>
       </c>
       <c r="F17">
-        <v>85.42532105817129</v>
+        <v>1116447.901494039</v>
       </c>
       <c r="G17">
-        <v>36.54422793183608</v>
+        <v>4841260.735504667</v>
       </c>
       <c r="H17">
-        <v>1649.12356064649</v>
+        <v>3985839.699923058</v>
       </c>
       <c r="I17">
-        <v>-606.9455664986425</v>
+        <v>1115392.330201359</v>
       </c>
       <c r="J17">
-        <v>980.0864850568469</v>
+        <v>4842480.428027861</v>
       </c>
       <c r="K17">
-        <v>3288.755051286672</v>
+        <v>3987328.200841533</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1031,22 +1031,22 @@
         <v>168.142</v>
       </c>
       <c r="F18">
-        <v>80.57206982796123</v>
+        <v>1116442.967929436</v>
       </c>
       <c r="G18">
-        <v>55.341758351161</v>
+        <v>4841277.248337759</v>
       </c>
       <c r="H18">
-        <v>1688.55452234093</v>
+        <v>3985874.784331376</v>
       </c>
       <c r="I18">
-        <v>-580.2672871769315</v>
+        <v>1115434.984807153</v>
       </c>
       <c r="J18">
-        <v>942.5476868575747</v>
+        <v>4842431.776570966</v>
       </c>
       <c r="K18">
-        <v>3373.643463503528</v>
+        <v>3987404.766760572</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1066,22 +1066,22 @@
         <v>169.142</v>
       </c>
       <c r="F19">
-        <v>76.45930457214168</v>
+        <v>1116438.78710464</v>
       </c>
       <c r="G19">
-        <v>74.13928877048596</v>
+        <v>4841293.761170849</v>
       </c>
       <c r="H19">
-        <v>1723.853167705663</v>
+        <v>3985906.191936817</v>
       </c>
       <c r="I19">
-        <v>-552.93207977049</v>
+        <v>1115478.689743373</v>
       </c>
       <c r="J19">
-        <v>905.0088886583026</v>
+        <v>4842383.125114069</v>
       </c>
       <c r="K19">
-        <v>3441.736635153434</v>
+        <v>3987466.184051007</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1101,22 +1101,22 @@
         <v>170.142</v>
       </c>
       <c r="F20">
-        <v>72.91655854713797</v>
+        <v>1116435.185731962</v>
       </c>
       <c r="G20">
-        <v>92.93681918981088</v>
+        <v>4841310.274003942</v>
       </c>
       <c r="H20">
-        <v>1755.804047980504</v>
+        <v>3985934.620807976</v>
       </c>
       <c r="I20">
-        <v>-524.9237680295946</v>
+        <v>1115523.470873439</v>
       </c>
       <c r="J20">
-        <v>867.4700904590305</v>
+        <v>4842334.473657173</v>
       </c>
       <c r="K20">
-        <v>3493.034566236391</v>
+        <v>3987512.452712837</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1136,22 +1136,22 @@
         <v>171.142</v>
       </c>
       <c r="F21">
-        <v>69.8235582074781</v>
+        <v>1116432.041547524</v>
       </c>
       <c r="G21">
-        <v>111.7343496091358</v>
+        <v>4841326.786837033</v>
       </c>
       <c r="H21">
-        <v>1784.987528891396</v>
+        <v>3985960.58733571</v>
       </c>
       <c r="I21">
-        <v>-496.2257773792541</v>
+        <v>1115569.354697635</v>
       </c>
       <c r="J21">
-        <v>829.9312922597584</v>
+        <v>4842285.822200278</v>
       </c>
       <c r="K21">
-        <v>3527.5372567524</v>
+        <v>3987543.572746063</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1171,22 +1171,22 @@
         <v>172.142</v>
       </c>
       <c r="F22">
-        <v>67.09273124127476</v>
+        <v>1116429.265529837</v>
       </c>
       <c r="G22">
-        <v>130.5318800284608</v>
+        <v>4841343.299670124</v>
       </c>
       <c r="H22">
-        <v>1811.845023312346</v>
+        <v>3985984.484275074</v>
       </c>
       <c r="I22">
-        <v>-466.8211251108161</v>
+        <v>1115616.36836879</v>
       </c>
       <c r="J22">
-        <v>792.3924940604863</v>
+        <v>4842237.170743382</v>
       </c>
       <c r="K22">
-        <v>3545.24470670146</v>
+        <v>3987559.544150684</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1206,22 +1206,22 @@
         <v>173.142</v>
       </c>
       <c r="F23">
-        <v>64.65861702574644</v>
+        <v>1116426.791135011</v>
       </c>
       <c r="G23">
-        <v>149.3294104477857</v>
+        <v>4841359.812503216</v>
       </c>
       <c r="H23">
-        <v>1836.72008936147</v>
+        <v>3986006.61731309</v>
       </c>
       <c r="I23">
-        <v>-436.6924103320518</v>
+        <v>1115664.539708346</v>
       </c>
       <c r="J23">
-        <v>754.8536958612142</v>
+        <v>4842188.519286486</v>
       </c>
       <c r="K23">
-        <v>3546.156916083571</v>
+        <v>3987560.366926702</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1241,22 +1241,22 @@
         <v>174.142</v>
       </c>
       <c r="F24">
-        <v>62.47118098587197</v>
+        <v>1116424.567500482</v>
       </c>
       <c r="G24">
-        <v>168.1269408671106</v>
+        <v>4841376.325336307</v>
       </c>
       <c r="H24">
-        <v>1859.885374645619</v>
+        <v>3986027.229042878</v>
       </c>
       <c r="I24">
-        <v>-405.82180366977</v>
+        <v>1115713.89722282</v>
       </c>
       <c r="J24">
-        <v>717.3148976619419</v>
+        <v>4842139.86782959</v>
       </c>
       <c r="K24">
-        <v>3530.273884898733</v>
+        <v>3987546.041074114</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1276,22 +1276,22 @@
         <v>175.142</v>
       </c>
       <c r="F25">
-        <v>60.4914410465818</v>
+        <v>1116422.554999084</v>
       </c>
       <c r="G25">
-        <v>186.9244712864356</v>
+        <v>4841392.838169399</v>
       </c>
       <c r="H25">
-        <v>1881.560880954617</v>
+        <v>3986046.515214992</v>
       </c>
       <c r="I25">
-        <v>-374.1910367188665</v>
+        <v>1115764.470120681</v>
       </c>
       <c r="J25">
-        <v>679.77609946267</v>
+        <v>4842091.216372694</v>
       </c>
       <c r="K25">
-        <v>3497.595613146947</v>
+        <v>3987516.566592922</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1311,22 +1311,22 @@
         <v>176.142</v>
       </c>
       <c r="F26">
-        <v>58.688518171862</v>
+        <v>1116420.722240783</v>
       </c>
       <c r="G26">
-        <v>205.7220017057605</v>
+        <v>4841409.35100249</v>
       </c>
       <c r="H26">
-        <v>1901.926702414066</v>
+        <v>3986064.636071424</v>
       </c>
       <c r="I26">
-        <v>-341.7813912315692</v>
+        <v>1115816.288329626</v>
       </c>
       <c r="J26">
-        <v>642.2373012633977</v>
+        <v>4842042.564915799</v>
       </c>
       <c r="K26">
-        <v>3448.122100828211</v>
+        <v>3987471.943483126</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1346,22 +1346,22 @@
         <v>177.142</v>
       </c>
       <c r="F27">
-        <v>57.03759414675821</v>
+        <v>1116419.043996665</v>
       </c>
       <c r="G27">
-        <v>224.5195321250854</v>
+        <v>4841425.863835581</v>
       </c>
       <c r="H27">
-        <v>1921.132129767381</v>
+        <v>3986081.7244463</v>
       </c>
       <c r="I27">
-        <v>-308.5736880404743</v>
+        <v>1115869.382514294</v>
       </c>
       <c r="J27">
-        <v>604.6985030641256</v>
+        <v>4841993.913458902</v>
       </c>
       <c r="K27">
-        <v>3381.853347942527</v>
+        <v>3987412.171744725</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1381,22 +1381,22 @@
         <v>178.142</v>
       </c>
       <c r="F28">
-        <v>55.51846455208186</v>
+        <v>1116417.49972796</v>
       </c>
       <c r="G28">
-        <v>243.3170625444104</v>
+        <v>4841442.376668673</v>
       </c>
       <c r="H28">
-        <v>1939.302297906912</v>
+        <v>3986097.891680647</v>
       </c>
       <c r="I28">
-        <v>-274.5482757088257</v>
+        <v>1115923.784094414</v>
       </c>
       <c r="J28">
-        <v>567.1597048648536</v>
+        <v>4841945.262002006</v>
       </c>
       <c r="K28">
-        <v>3298.789354489895</v>
+        <v>3987337.25137772</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1416,22 +1416,22 @@
         <v>179.142</v>
       </c>
       <c r="F29">
-        <v>54.11449240158025</v>
+        <v>1116416.072522365</v>
       </c>
       <c r="G29">
-        <v>262.1145929637353</v>
+        <v>4841458.889501764</v>
       </c>
       <c r="H29">
-        <v>1956.543131614325</v>
+        <v>3986113.232022945</v>
       </c>
       <c r="I29">
-        <v>-239.6850189013152</v>
+        <v>1115979.525263395</v>
       </c>
       <c r="J29">
-        <v>529.6209066655814</v>
+        <v>4841896.610545111</v>
       </c>
       <c r="K29">
-        <v>3198.930120470313</v>
+        <v>3987247.182382111</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1451,22 +1451,22 @@
         <v>180.142</v>
       </c>
       <c r="F30">
-        <v>52.8118377074324</v>
+        <v>1116414.748310867</v>
       </c>
       <c r="G30">
-        <v>280.9121233830602</v>
+        <v>4841475.402334856</v>
       </c>
       <c r="H30">
-        <v>1972.945086941199</v>
+        <v>3986127.825958096</v>
       </c>
       <c r="I30">
-        <v>-203.963286468528</v>
+        <v>1116036.639007382</v>
       </c>
       <c r="J30">
-        <v>492.0821084663092</v>
+        <v>4841847.959088216</v>
       </c>
       <c r="K30">
-        <v>3082.275645883783</v>
+        <v>3987141.964757897</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1486,22 +1486,22 @@
         <v>181.142</v>
       </c>
       <c r="F31">
-        <v>51.59888096950716</v>
+        <v>1116413.515281678</v>
       </c>
       <c r="G31">
-        <v>299.7096538023852</v>
+        <v>4841491.915167947</v>
       </c>
       <c r="H31">
-        <v>1988.586023880486</v>
+        <v>3986141.74276343</v>
       </c>
       <c r="I31">
-        <v>-167.3619392379748</v>
+        <v>1116095.15912477</v>
       </c>
       <c r="J31">
-        <v>454.5433102670372</v>
+        <v>4841799.307631318</v>
       </c>
       <c r="K31">
-        <v>2948.825930730305</v>
+        <v>3987021.598505079</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1521,22 +1521,22 @@
         <v>182.142</v>
       </c>
       <c r="F32">
-        <v>50.46578545869149</v>
+        <v>1116412.363435289</v>
       </c>
       <c r="G32">
-        <v>318.5071842217101</v>
+        <v>4841508.428001039</v>
       </c>
       <c r="H32">
-        <v>2003.533441671419</v>
+        <v>3986155.042497613</v>
       </c>
       <c r="I32">
-        <v>-129.8593175044912</v>
+        <v>1116155.120246212</v>
       </c>
       <c r="J32">
-        <v>417.004512067765</v>
+        <v>4841750.656174423</v>
       </c>
       <c r="K32">
-        <v>2798.580975009877</v>
+        <v>3986886.083623656</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1556,22 +1556,22 @@
         <v>183.142</v>
       </c>
       <c r="F33">
-        <v>49.40416048096623</v>
+        <v>1116411.284242154</v>
       </c>
       <c r="G33">
-        <v>337.304714641035</v>
+        <v>4841524.94083413</v>
       </c>
       <c r="H33">
-        <v>2017.846239248782</v>
+        <v>3986167.77756703</v>
       </c>
       <c r="I33">
-        <v>-91.43322821259972</v>
+        <v>1116216.557855106</v>
       </c>
       <c r="J33">
-        <v>379.465713868493</v>
+        <v>4841702.004717528</v>
       </c>
       <c r="K33">
-        <v>2631.5407787225</v>
+        <v>3986735.420113629</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1591,22 +1591,22 @@
         <v>184.142</v>
       </c>
       <c r="F34">
-        <v>48.40679921180181</v>
+        <v>1116410.270376187</v>
       </c>
       <c r="G34">
-        <v>356.10224506036</v>
+        <v>4841541.453667222</v>
       </c>
       <c r="H34">
-        <v>2031.576116969891</v>
+        <v>3986179.993973007</v>
       </c>
       <c r="I34">
-        <v>-52.06093182324929</v>
+        <v>1116279.508308598</v>
       </c>
       <c r="J34">
-        <v>341.9269156692208</v>
+        <v>4841653.353260632</v>
       </c>
       <c r="K34">
-        <v>2447.705341868175</v>
+        <v>3986569.607974997</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1626,22 +1626,22 @@
         <v>185.142</v>
       </c>
       <c r="F35">
-        <v>47.46747234865585</v>
+        <v>1116409.315505</v>
       </c>
       <c r="G35">
-        <v>374.8997754796849</v>
+        <v>4841557.966500313</v>
       </c>
       <c r="H35">
-        <v>2044.768703910401</v>
+        <v>3986191.732314836</v>
       </c>
       <c r="I35">
-        <v>-11.71912885715978</v>
+        <v>1116344.008859093</v>
       </c>
       <c r="J35">
-        <v>304.3881174699487</v>
+        <v>4841604.701803735</v>
       </c>
       <c r="K35">
-        <v>2247.074664446901</v>
+        <v>3986388.647207761</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1661,22 +1661,22 @@
         <v>186.142</v>
       </c>
       <c r="F36">
-        <v>46.58076406555679</v>
+        <v>1116408.414123144</v>
       </c>
       <c r="G36">
-        <v>393.6973058990098</v>
+        <v>4841574.479333404</v>
       </c>
       <c r="H36">
-        <v>2057.464472780845</v>
+        <v>3986203.028603839</v>
       </c>
       <c r="I36">
-        <v>29.6160538931916</v>
+        <v>1116410.097676305</v>
       </c>
       <c r="J36">
-        <v>266.8493192706766</v>
+        <v>4841556.05034684</v>
       </c>
       <c r="K36">
-        <v>2029.648746458678</v>
+        <v>3986192.537811921</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1696,22 +1696,22 @@
         <v>187.142</v>
       </c>
       <c r="F37">
-        <v>45.74194039303693</v>
+        <v>1116407.561418312</v>
       </c>
       <c r="G37">
-        <v>412.4948363183348</v>
+        <v>4841590.992166496</v>
       </c>
       <c r="H37">
-        <v>2069.699488739484</v>
+        <v>3986213.91492964</v>
       </c>
       <c r="I37">
-        <v>71.96907749109948</v>
+        <v>1116477.81386984</v>
       </c>
       <c r="J37">
-        <v>229.3105210714045</v>
+        <v>4841507.398889944</v>
       </c>
       <c r="K37">
-        <v>1795.427587903507</v>
+        <v>3985981.279787476</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1731,22 +1731,22 @@
         <v>188.142</v>
       </c>
       <c r="F38">
-        <v>44.94684271427849</v>
+        <v>1116406.753163066</v>
       </c>
       <c r="G38">
-        <v>431.2923667376597</v>
+        <v>4841607.504999587</v>
       </c>
       <c r="H38">
-        <v>2081.506027024582</v>
+        <v>3986224.420009715</v>
       </c>
       <c r="I38">
-        <v>115.365005331039</v>
+        <v>1116547.197512344</v>
       </c>
       <c r="J38">
-        <v>191.7717228721324</v>
+        <v>4841458.747433049</v>
       </c>
       <c r="K38">
-        <v>1544.411188781388</v>
+        <v>3985754.873134427</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1766,22 +1766,22 @@
         <v>189.142</v>
       </c>
       <c r="F39">
-        <v>44.19180090505635</v>
+        <v>1116405.98562655</v>
       </c>
       <c r="G39">
-        <v>450.0898971569846</v>
+        <v>4841624.017832679</v>
       </c>
       <c r="H39">
-        <v>2092.913086052129</v>
+        <v>3986234.569645925</v>
       </c>
       <c r="I39">
-        <v>159.829517970515</v>
+        <v>1116618.289663212</v>
       </c>
       <c r="J39">
-        <v>154.2329246728603</v>
+        <v>4841410.095976152</v>
       </c>
       <c r="K39">
-        <v>1276.599549092318</v>
+        <v>3985513.317852773</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1801,22 +1801,22 @@
         <v>190.142</v>
       </c>
       <c r="F40">
-        <v>43.47356197580844</v>
+        <v>1116405.255501941</v>
       </c>
       <c r="G40">
-        <v>468.8874275763096</v>
+        <v>4841640.530665771</v>
       </c>
       <c r="H40">
-        <v>2103.94681651673</v>
+        <v>3986244.387106324</v>
       </c>
       <c r="I40">
-        <v>205.3889283271369</v>
+        <v>1116691.132392892</v>
       </c>
       <c r="J40">
-        <v>116.6941264735881</v>
+        <v>4841361.444519256</v>
       </c>
       <c r="K40">
-        <v>991.9926688363</v>
+        <v>3985256.613942515</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1836,22 +1836,22 @@
         <v>191.142</v>
       </c>
       <c r="F41">
-        <v>42.78923104978382</v>
+        <v>1116404.559846457</v>
       </c>
       <c r="G41">
-        <v>487.6849579956345</v>
+        <v>4841657.043498862</v>
       </c>
       <c r="H41">
-        <v>2114.630882474745</v>
+        <v>3986253.893446429</v>
       </c>
       <c r="I41">
-        <v>252.070197249901</v>
+        <v>1116765.768807776</v>
       </c>
       <c r="J41">
-        <v>79.15532827431608</v>
+        <v>4841312.793062361</v>
       </c>
       <c r="K41">
-        <v>690.5905480133341</v>
+        <v>3984984.761403653</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1871,22 +1871,22 @@
         <v>192.142</v>
       </c>
       <c r="F42">
-        <v>42.13622223438527</v>
+        <v>1116403.896031413</v>
       </c>
       <c r="G42">
-        <v>506.4824884149594</v>
+        <v>4841673.556331953</v>
       </c>
       <c r="H42">
-        <v>2124.986766951072</v>
+        <v>3986263.107781152</v>
       </c>
       <c r="I42">
-        <v>299.9009494739092</v>
+        <v>1116842.243075712</v>
       </c>
       <c r="J42">
-        <v>41.61653007504389</v>
+        <v>4841264.141605466</v>
       </c>
       <c r="K42">
-        <v>372.3931866234185</v>
+        <v>3984697.760236186</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1906,22 +1906,22 @@
         <v>193.142</v>
       </c>
       <c r="F43">
-        <v>41.51221748435822</v>
+        <v>1116403.261700405</v>
       </c>
       <c r="G43">
-        <v>525.2800188342844</v>
+        <v>4841690.069165045</v>
       </c>
       <c r="H43">
-        <v>2135.034031993377</v>
+        <v>3986272.047516174</v>
       </c>
       <c r="I43">
-        <v>348.9094899679481</v>
+        <v>1116920.600452141</v>
       </c>
       <c r="J43">
-        <v>4.077731875771707</v>
+        <v>4841215.490148569</v>
       </c>
       <c r="K43">
-        <v>37.40058466655433</v>
+        <v>3984395.610440115</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1941,22 +1941,22 @@
         <v>194.142</v>
       </c>
       <c r="F44">
-        <v>40.91513196490486</v>
+        <v>1116402.654734097</v>
       </c>
       <c r="G44">
-        <v>544.0775492536093</v>
+        <v>4841706.581998136</v>
       </c>
       <c r="H44">
-        <v>2144.790541086315</v>
+        <v>3986280.728545854</v>
       </c>
       <c r="I44">
-        <v>399.1248206846217</v>
+        <v>1117000.887306877</v>
       </c>
       <c r="J44">
-        <v>-33.4610663235003</v>
+        <v>4841166.838691673</v>
       </c>
       <c r="K44">
-        <v>-314.3872578572576</v>
+        <v>3984078.312015438</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1976,22 +1976,22 @@
         <v>195.142</v>
       </c>
       <c r="F45">
-        <v>40.34308473511875</v>
+        <v>1116402.073220421</v>
       </c>
       <c r="G45">
-        <v>562.8750796729342</v>
+        <v>4841723.094831228</v>
       </c>
       <c r="H45">
-        <v>2154.272650279826</v>
+        <v>3986289.165423281</v>
       </c>
       <c r="I45">
-        <v>450.5766577229365</v>
+        <v>1117083.151151549</v>
       </c>
       <c r="J45">
-        <v>-70.99986452277248</v>
+        <v>4841118.187234778</v>
       </c>
       <c r="K45">
-        <v>-682.9703409480193</v>
+        <v>3983745.864962159</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2011,22 +2011,22 @@
         <v>196.142</v>
       </c>
       <c r="F46">
-        <v>39.79437381238048</v>
+        <v>1116401.515429229</v>
       </c>
       <c r="G46">
-        <v>581.6726100922592</v>
+        <v>4841739.607664319</v>
       </c>
       <c r="H46">
-        <v>2163.495373168303</v>
+        <v>3986297.371507072</v>
       </c>
       <c r="I46">
-        <v>503.295448913498</v>
+        <v>1117167.440667714</v>
       </c>
       <c r="J46">
-        <v>-108.5386627220447</v>
+        <v>4841069.535777881</v>
       </c>
       <c r="K46">
-        <v>-1068.348664605731</v>
+        <v>3983398.269280274</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2046,22 +2046,22 @@
         <v>197.142</v>
       </c>
       <c r="F47">
-        <v>39.26745486462884</v>
+        <v>1116400.979790635</v>
       </c>
       <c r="G47">
-        <v>600.4701405115841</v>
+        <v>4841756.12049741</v>
       </c>
       <c r="H47">
-        <v>2172.472523899653</v>
+        <v>3986305.359088614</v>
       </c>
       <c r="I47">
-        <v>557.3123918367285</v>
+        <v>1117253.80573567</v>
       </c>
       <c r="J47">
-        <v>-146.0774609213169</v>
+        <v>4841020.884320986</v>
       </c>
       <c r="K47">
-        <v>-1470.52222883039</v>
+        <v>3983035.524969785</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2081,22 +2081,22 @@
         <v>198.142</v>
       </c>
       <c r="F48">
-        <v>38.76092292291384</v>
+        <v>1116400.464876418</v>
       </c>
       <c r="G48">
-        <v>619.267670930909</v>
+        <v>4841772.633330503</v>
       </c>
       <c r="H48">
-        <v>2181.216841634243</v>
+        <v>3986313.139502803</v>
       </c>
       <c r="I48">
-        <v>612.659452284767</v>
+        <v>1117342.29746397</v>
       </c>
       <c r="J48">
-        <v>-183.6162591205887</v>
+        <v>4840972.23286409</v>
       </c>
       <c r="K48">
-        <v>-1889.491033621995</v>
+        <v>3982657.632030691</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2116,22 +2116,22 @@
         <v>199.142</v>
       </c>
       <c r="F49">
-        <v>38.27349662108366</v>
+        <v>1116399.969384007</v>
       </c>
       <c r="G49">
-        <v>638.065201350234</v>
+        <v>4841789.146163593</v>
       </c>
       <c r="H49">
-        <v>2189.740099268272</v>
+        <v>3986320.723224787</v>
       </c>
       <c r="I49">
-        <v>669.3693831779771</v>
+        <v>1117432.968219669</v>
       </c>
       <c r="J49">
-        <v>-221.1550573198609</v>
+        <v>4840923.581407194</v>
       </c>
       <c r="K49">
-        <v>-2325.255078980552</v>
+        <v>3982264.590462994</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2151,22 +2151,22 @@
         <v>200.142</v>
       </c>
       <c r="F50">
-        <v>37.80400456007234</v>
+        <v>1116399.492122621</v>
       </c>
       <c r="G50">
-        <v>656.8627317695589</v>
+        <v>4841805.658996685</v>
       </c>
       <c r="H50">
-        <v>2198.053198750214</v>
+        <v>3986328.119954769</v>
       </c>
       <c r="I50">
-        <v>727.4757439472522</v>
+        <v>1117525.871659311</v>
       </c>
       <c r="J50">
-        <v>-258.6938555191331</v>
+        <v>4840874.929950298</v>
       </c>
       <c r="K50">
-        <v>-2777.814364906058</v>
+        <v>3981856.400266692</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2186,22 +2186,22 @@
         <v>201.142</v>
       </c>
       <c r="F51">
-        <v>37.35137346645489</v>
+        <v>1116399.032001222</v>
       </c>
       <c r="G51">
-        <v>675.6602621888838</v>
+        <v>4841822.171829777</v>
       </c>
       <c r="H51">
-        <v>2206.166254926533</v>
+        <v>3986335.338692618</v>
       </c>
       <c r="I51">
-        <v>787.0129203935991</v>
+        <v>1117621.062760684</v>
       </c>
       <c r="J51">
-        <v>-296.2326537184052</v>
+        <v>4840826.278493403</v>
       </c>
       <c r="K51">
-        <v>-3247.168891398513</v>
+        <v>3981433.061441785</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2221,22 +2221,22 @@
         <v>202.142</v>
       </c>
       <c r="F52">
-        <v>36.91461787280625</v>
+        <v>1116398.588018038</v>
       </c>
       <c r="G52">
-        <v>694.4577926082088</v>
+        <v>4841838.684662867</v>
       </c>
       <c r="H52">
-        <v>2214.088669534348</v>
+        <v>3986342.387803698</v>
       </c>
       <c r="I52">
-        <v>848.0161450367399</v>
+        <v>1117718.597855355</v>
       </c>
       <c r="J52">
-        <v>-333.7714519176774</v>
+        <v>4840777.627036506</v>
       </c>
       <c r="K52">
-        <v>-3733.318658457915</v>
+        <v>3980994.573988274</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2256,22 +2256,22 @@
         <v>203.142</v>
       </c>
       <c r="F53">
-        <v>36.49283109404057</v>
+        <v>1116398.159251378</v>
       </c>
       <c r="G53">
-        <v>713.2553230275337</v>
+        <v>4841855.19749596</v>
       </c>
       <c r="H53">
-        <v>2221.829196698628</v>
+        <v>3986349.275077149</v>
       </c>
       <c r="I53">
-        <v>910.521517964779</v>
+        <v>1117818.534662001</v>
       </c>
       <c r="J53">
-        <v>-371.3102501169492</v>
+        <v>4840728.975579611</v>
       </c>
       <c r="K53">
-        <v>-4236.263666084264</v>
+        <v>3980540.937906159</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2291,22 +2291,22 @@
         <v>204.142</v>
       </c>
       <c r="F54">
-        <v>36.08517731170664</v>
+        <v>1116397.744851592</v>
       </c>
       <c r="G54">
-        <v>732.0528534468586</v>
+        <v>4841871.710329051</v>
       </c>
       <c r="H54">
-        <v>2229.396001078201</v>
+        <v>3986356.007777624</v>
       </c>
       <c r="I54">
-        <v>974.5660281972836</v>
+        <v>1117920.932320571</v>
       </c>
       <c r="J54">
-        <v>-408.8490483162215</v>
+        <v>4840680.324122714</v>
       </c>
       <c r="K54">
-        <v>-4756.003914277565</v>
+        <v>3980072.153195439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>